<commit_message>
Finished random question at registration page
</commit_message>
<xml_diff>
--- a/synergy-bank/src/main/webapp/WEB-INF/files/security_questions.xlsx
+++ b/synergy-bank/src/main/webapp/WEB-INF/files/security_questions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>What is your birth place?</t>
   </si>
@@ -46,6 +46,36 @@
   </si>
   <si>
     <t>What is your favorite soccer team?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q006 </t>
+  </si>
+  <si>
+    <t>What is the name of your favorite childhood hero?</t>
+  </si>
+  <si>
+    <t>Q007</t>
+  </si>
+  <si>
+    <t>What is your fathers middle name?</t>
+  </si>
+  <si>
+    <t>Q008</t>
+  </si>
+  <si>
+    <t>What is the name of your first school?</t>
+  </si>
+  <si>
+    <t>Q009</t>
+  </si>
+  <si>
+    <t>What is the name of your fist crush?</t>
+  </si>
+  <si>
+    <t>Q010</t>
+  </si>
+  <si>
+    <t>What is the registration number of your first vehicle?</t>
   </si>
 </sst>
 </file>
@@ -377,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -426,6 +456,46 @@
       </c>
       <c r="B5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>